<commit_message>
Added higher tier score achievements
</commit_message>
<xml_diff>
--- a/My Sets/Armor Attack (Vectrex)/Armor Attack - Plan.xlsx
+++ b/My Sets/Armor Attack (Vectrex)/Armor Attack - Plan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egrea\Dropbox\RetroArch\Achievements\Armor..Attack\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Dropbox\RetroArch\Achievements\Armor..Attack\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23250" windowHeight="12570" tabRatio="635"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="635"/>
   </bookViews>
   <sheets>
     <sheet name="Achievements" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Game Dec" sheetId="16" state="hidden" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Achievements!$B$1:$G$185</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Achievements!$B$1:$G$187</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Checklist!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Extras!$A$1:$F$53</definedName>
   </definedNames>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="108">
   <si>
     <t>Description</t>
   </si>
@@ -187,9 +187,6 @@
     <t>Fully destroy 10 tanks (requires two shots)</t>
   </si>
   <si>
-    <t>Fully destroy 25 tanks (requires two shots)</t>
-  </si>
-  <si>
     <t>King of the Hill</t>
   </si>
   <si>
@@ -262,9 +259,6 @@
     <t>Corporal </t>
   </si>
   <si>
-    <t>Get to the Chopper!</t>
-  </si>
-  <si>
     <t>Blackhawk Down!</t>
   </si>
   <si>
@@ -313,9 +307,6 @@
     <t>Reach the final speed up phase in mode 3</t>
   </si>
   <si>
-    <t>Fully destroy 50 tanks (requires two shots)</t>
-  </si>
-  <si>
     <t>Destroy 6 Helicoptors</t>
   </si>
   <si>
@@ -359,6 +350,24 @@
   </si>
   <si>
     <t>Let an enemy damage or destroy another tank 25 times</t>
+  </si>
+  <si>
+    <t>Aerial Attack!</t>
+  </si>
+  <si>
+    <t>Fully destroy 20 tanks (requires two shots)</t>
+  </si>
+  <si>
+    <t>Fully destroy 30 tanks (requires two shots)</t>
+  </si>
+  <si>
+    <t>Score 100,000</t>
+  </si>
+  <si>
+    <t>Sergeant Major</t>
+  </si>
+  <si>
+    <t>Indestructible</t>
   </si>
 </sst>
 </file>
@@ -727,25 +736,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G185"/>
+  <dimension ref="A1:G187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E2:E23"/>
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" customWidth="1"/>
-    <col min="5" max="5" width="8.453125" customWidth="1"/>
-    <col min="6" max="6" width="84.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="84.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="e">
         <f>CHAR(34)+Achievements!#REF!+CHAR(34)+","+CHAR(34)</f>
         <v>#VALUE!</v>
@@ -769,7 +778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -777,7 +786,7 @@
         <v>44</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>10</v>
@@ -791,7 +800,7 @@
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -799,7 +808,7 @@
         <v>44</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>12</v>
@@ -809,11 +818,11 @@
         <v>5</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -821,7 +830,7 @@
         <v>44</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>13</v>
@@ -835,29 +844,29 @@
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" s="7" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>95</v>
+        <v>44</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>106</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E5" s="7">
         <f>VLOOKUP(D5,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -865,21 +874,21 @@
         <v>35</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="7">
         <f>VLOOKUP(D6,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -887,21 +896,21 @@
         <v>35</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="7">
         <f>VLOOKUP(D7,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -909,21 +918,21 @@
         <v>35</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" s="7">
         <f>VLOOKUP(D8,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -931,7 +940,7 @@
         <v>35</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>12</v>
@@ -941,11 +950,11 @@
         <v>5</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -953,7 +962,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>12</v>
@@ -963,13 +972,11 @@
         <v>5</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -977,23 +984,21 @@
         <v>35</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E11" s="7">
         <f>VLOOKUP(D11,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -1001,7 +1006,7 @@
         <v>35</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>12</v>
@@ -1011,13 +1016,13 @@
         <v>5</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -1025,21 +1030,23 @@
         <v>35</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E13" s="7">
         <f>VLOOKUP(D13,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -1047,7 +1054,7 @@
         <v>35</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>12</v>
@@ -1057,11 +1064,13 @@
         <v>5</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -1069,7 +1078,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>17</v>
@@ -1079,11 +1088,11 @@
         <v>2</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -1091,7 +1100,7 @@
         <v>35</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>12</v>
@@ -1101,11 +1110,11 @@
         <v>5</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -1113,65 +1122,65 @@
         <v>35</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E17" s="7">
         <f>VLOOKUP(D17,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E18" s="7">
         <f>VLOOKUP(D18,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E19" s="7">
         <f>VLOOKUP(D19,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>19</v>
       </c>
@@ -1179,21 +1188,21 @@
         <v>38</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E20" s="7">
         <f>VLOOKUP(D20,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>20</v>
       </c>
@@ -1201,21 +1210,21 @@
         <v>38</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E21" s="7">
         <f>VLOOKUP(D21,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -1223,21 +1232,21 @@
         <v>38</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E22" s="7">
         <f>VLOOKUP(D22,Stats!$A$1:$B$10,2,FALSE)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>22</v>
       </c>
@@ -1245,955 +1254,999 @@
         <v>38</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E23" s="7">
         <f>VLOOKUP(D23,Stats!$A$1:$B$10,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>23</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="7">
+        <f>VLOOKUP(D24,Stats!$A$1:$B$10,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>24</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="7">
+        <f>VLOOKUP(D25,Stats!$A$1:$B$10,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="8"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="8"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="F25" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="8"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="8"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="8"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="8"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="8"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="8"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="8"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="G36" s="5"/>
     </row>
-    <row r="37" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="G37" s="5"/>
     </row>
-    <row r="38" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="8"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="41" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="8"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="8"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="8"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="G43" s="5"/>
     </row>
-    <row r="44" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="8"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="G44" s="5"/>
     </row>
-    <row r="45" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="8"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="8"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="G47" s="5"/>
     </row>
-    <row r="48" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="G48" s="5"/>
     </row>
-    <row r="49" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="G49" s="5"/>
     </row>
-    <row r="50" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="8"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="G50" s="5"/>
     </row>
-    <row r="51" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="8"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="G51" s="5"/>
     </row>
-    <row r="52" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="8"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
-      <c r="E52" s="7">
-        <f>SUM(E2:E51)</f>
-        <v>100</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>42</v>
-      </c>
       <c r="G52" s="5"/>
     </row>
-    <row r="53" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="G53" s="5"/>
     </row>
-    <row r="54" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="8"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
+      <c r="E54" s="7">
+        <f>SUM(E2:E53)</f>
+        <v>135</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="G54" s="5"/>
     </row>
-    <row r="55" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="8"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="G55" s="5"/>
     </row>
-    <row r="56" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="8"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="G56" s="5"/>
     </row>
-    <row r="57" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="8"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="G57" s="5"/>
     </row>
-    <row r="58" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="8"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="G58" s="5"/>
     </row>
-    <row r="59" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="8"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="G59" s="5"/>
     </row>
-    <row r="60" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="8"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
       <c r="G60" s="5"/>
     </row>
-    <row r="61" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="8"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="G61" s="5"/>
     </row>
-    <row r="62" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="8"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="G62" s="5"/>
     </row>
-    <row r="63" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="8"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="G63" s="5"/>
     </row>
-    <row r="64" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
-      <c r="C64" s="10"/>
+      <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="G64" s="5"/>
     </row>
-    <row r="65" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="8"/>
-      <c r="C65" s="10"/>
+      <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="G65" s="5"/>
     </row>
-    <row r="66" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="8"/>
       <c r="C66" s="10"/>
       <c r="D66" s="5"/>
       <c r="G66" s="5"/>
     </row>
-    <row r="67" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="8"/>
       <c r="C67" s="10"/>
       <c r="D67" s="5"/>
       <c r="G67" s="5"/>
     </row>
-    <row r="68" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="8"/>
       <c r="C68" s="10"/>
       <c r="D68" s="5"/>
       <c r="G68" s="5"/>
     </row>
-    <row r="69" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="8"/>
       <c r="C69" s="10"/>
       <c r="D69" s="5"/>
       <c r="G69" s="5"/>
     </row>
-    <row r="70" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="8"/>
-      <c r="C70" s="5"/>
+      <c r="C70" s="10"/>
       <c r="D70" s="5"/>
       <c r="G70" s="5"/>
     </row>
-    <row r="71" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="8"/>
-      <c r="C71" s="5"/>
+      <c r="C71" s="10"/>
       <c r="D71" s="5"/>
       <c r="G71" s="5"/>
     </row>
-    <row r="72" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="8"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="G72" s="5"/>
     </row>
-    <row r="73" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="8"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="G73" s="5"/>
     </row>
-    <row r="74" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="8"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="G74" s="5"/>
     </row>
-    <row r="75" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="8"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="G75" s="5"/>
     </row>
-    <row r="76" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="8"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
       <c r="G76" s="5"/>
     </row>
-    <row r="77" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="8"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
       <c r="G77" s="5"/>
     </row>
-    <row r="78" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="8"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
       <c r="G78" s="5"/>
     </row>
-    <row r="79" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="8"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="G79" s="5"/>
     </row>
-    <row r="80" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="8"/>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="G80" s="5"/>
     </row>
-    <row r="81" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="8"/>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="G81" s="5"/>
     </row>
-    <row r="82" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="8"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="G82" s="5"/>
     </row>
-    <row r="83" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="8"/>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
       <c r="G83" s="5"/>
     </row>
-    <row r="84" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="8"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
       <c r="G84" s="5"/>
     </row>
-    <row r="85" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="8"/>
-      <c r="C85" s="10"/>
+      <c r="C85" s="5"/>
       <c r="D85" s="5"/>
       <c r="G85" s="5"/>
     </row>
-    <row r="86" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B86" s="8"/>
-      <c r="C86" s="10"/>
+      <c r="C86" s="5"/>
       <c r="D86" s="5"/>
       <c r="G86" s="5"/>
     </row>
-    <row r="87" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B87" s="8"/>
       <c r="C87" s="10"/>
       <c r="D87" s="5"/>
       <c r="G87" s="5"/>
     </row>
-    <row r="88" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="8"/>
       <c r="C88" s="10"/>
       <c r="D88" s="5"/>
       <c r="G88" s="5"/>
     </row>
-    <row r="89" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="8"/>
       <c r="C89" s="10"/>
       <c r="D89" s="5"/>
       <c r="G89" s="5"/>
     </row>
-    <row r="90" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="8"/>
       <c r="C90" s="10"/>
       <c r="D90" s="5"/>
       <c r="G90" s="5"/>
     </row>
-    <row r="91" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="8"/>
       <c r="C91" s="10"/>
       <c r="D91" s="5"/>
       <c r="G91" s="5"/>
     </row>
-    <row r="92" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B92" s="8"/>
       <c r="C92" s="10"/>
       <c r="D92" s="5"/>
       <c r="G92" s="5"/>
     </row>
-    <row r="93" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="8"/>
       <c r="C93" s="10"/>
       <c r="D93" s="5"/>
       <c r="G93" s="5"/>
     </row>
-    <row r="94" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B94" s="8"/>
       <c r="C94" s="10"/>
       <c r="D94" s="5"/>
       <c r="G94" s="5"/>
     </row>
-    <row r="95" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="8"/>
       <c r="C95" s="10"/>
       <c r="D95" s="5"/>
       <c r="G95" s="5"/>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B96" s="8"/>
       <c r="C96" s="10"/>
       <c r="D96" s="5"/>
-      <c r="E96" s="7"/>
-      <c r="F96" s="7"/>
-    </row>
-    <row r="97" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G96" s="5"/>
+    </row>
+    <row r="97" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B97" s="8"/>
       <c r="C97" s="10"/>
       <c r="D97" s="5"/>
       <c r="G97" s="5"/>
     </row>
-    <row r="98" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" s="8"/>
       <c r="C98" s="10"/>
       <c r="D98" s="5"/>
-      <c r="G98" s="5"/>
-    </row>
-    <row r="99" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E98" s="7"/>
+      <c r="F98" s="7"/>
+    </row>
+    <row r="99" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B99" s="8"/>
       <c r="C99" s="10"/>
       <c r="D99" s="5"/>
       <c r="G99" s="5"/>
     </row>
-    <row r="100" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B100" s="8"/>
-      <c r="C100" s="5"/>
+      <c r="C100" s="10"/>
       <c r="D100" s="5"/>
-    </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G100" s="5"/>
+    </row>
+    <row r="101" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="8"/>
       <c r="C101" s="10"/>
       <c r="D101" s="5"/>
-      <c r="E101" s="7"/>
-      <c r="F101" s="7"/>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="F102" s="7"/>
-    </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G101" s="5"/>
+    </row>
+    <row r="102" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="8"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B103" s="8"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="7"/>
       <c r="F103" s="7"/>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F104" s="7"/>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F105" s="7"/>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F106" s="7"/>
     </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F107" s="7"/>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F108" s="7"/>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F109" s="7"/>
     </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B110" s="8"/>
-      <c r="C110" s="10"/>
-      <c r="D110" s="5"/>
-      <c r="E110" s="7"/>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F110" s="7"/>
     </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B111" s="8"/>
-      <c r="C111" s="10"/>
-      <c r="D111" s="5"/>
-      <c r="E111" s="7"/>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F111" s="7"/>
     </row>
-    <row r="112" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B112" s="8"/>
       <c r="C112" s="10"/>
       <c r="D112" s="5"/>
-      <c r="G112" s="5"/>
-    </row>
-    <row r="113" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E112" s="7"/>
+      <c r="F112" s="7"/>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B113" s="8"/>
       <c r="C113" s="10"/>
       <c r="D113" s="5"/>
-      <c r="G113" s="5"/>
-    </row>
-    <row r="114" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E113" s="7"/>
+      <c r="F113" s="7"/>
+    </row>
+    <row r="114" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B114" s="8"/>
-      <c r="C114" s="5"/>
+      <c r="C114" s="10"/>
       <c r="D114" s="5"/>
       <c r="G114" s="5"/>
     </row>
-    <row r="115" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B115" s="8"/>
-      <c r="C115" s="5"/>
+      <c r="C115" s="10"/>
       <c r="D115" s="5"/>
       <c r="G115" s="5"/>
     </row>
-    <row r="116" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B116" s="8"/>
       <c r="C116" s="5"/>
       <c r="D116" s="5"/>
       <c r="G116" s="5"/>
     </row>
-    <row r="117" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B117" s="8"/>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
-      <c r="E117" s="5"/>
       <c r="G117" s="5"/>
     </row>
-    <row r="118" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B118" s="8"/>
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
-      <c r="E118" s="5"/>
       <c r="G118" s="5"/>
     </row>
-    <row r="119" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B119" s="8"/>
       <c r="C119" s="5"/>
       <c r="D119" s="5"/>
       <c r="E119" s="5"/>
       <c r="G119" s="5"/>
     </row>
-    <row r="120" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B120" s="8"/>
       <c r="C120" s="5"/>
       <c r="D120" s="5"/>
       <c r="E120" s="5"/>
       <c r="G120" s="5"/>
     </row>
-    <row r="121" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B121" s="8"/>
       <c r="C121" s="5"/>
       <c r="D121" s="5"/>
       <c r="E121" s="5"/>
       <c r="G121" s="5"/>
     </row>
-    <row r="122" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B122" s="8"/>
       <c r="C122" s="5"/>
       <c r="D122" s="5"/>
       <c r="E122" s="5"/>
       <c r="G122" s="5"/>
     </row>
-    <row r="123" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B123" s="8"/>
       <c r="C123" s="5"/>
       <c r="D123" s="5"/>
       <c r="E123" s="5"/>
       <c r="G123" s="5"/>
     </row>
-    <row r="124" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B124" s="8"/>
       <c r="C124" s="5"/>
       <c r="D124" s="5"/>
       <c r="E124" s="5"/>
       <c r="G124" s="5"/>
     </row>
-    <row r="125" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B125" s="8"/>
       <c r="C125" s="5"/>
       <c r="D125" s="5"/>
       <c r="E125" s="5"/>
       <c r="G125" s="5"/>
     </row>
-    <row r="126" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B126" s="8"/>
       <c r="C126" s="5"/>
       <c r="D126" s="5"/>
       <c r="E126" s="5"/>
       <c r="G126" s="5"/>
     </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B127" s="8"/>
+      <c r="C127" s="5"/>
       <c r="D127" s="5"/>
       <c r="E127" s="5"/>
-      <c r="F127" s="7"/>
       <c r="G127" s="5"/>
     </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B128" s="8"/>
+      <c r="C128" s="5"/>
       <c r="D128" s="5"/>
       <c r="E128" s="5"/>
-      <c r="F128" s="7"/>
       <c r="G128" s="5"/>
     </row>
-    <row r="129" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B129" s="8"/>
-      <c r="C129" s="5"/>
       <c r="D129" s="5"/>
       <c r="E129" s="5"/>
+      <c r="F129" s="7"/>
       <c r="G129" s="5"/>
     </row>
-    <row r="130" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" s="8"/>
-      <c r="C130" s="5"/>
       <c r="D130" s="5"/>
       <c r="E130" s="5"/>
-      <c r="G130" s="9"/>
-    </row>
-    <row r="131" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F130" s="7"/>
+      <c r="G130" s="5"/>
+    </row>
+    <row r="131" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B131" s="8"/>
       <c r="C131" s="5"/>
       <c r="D131" s="5"/>
       <c r="E131" s="5"/>
       <c r="G131" s="5"/>
     </row>
-    <row r="132" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B132" s="8"/>
       <c r="C132" s="5"/>
       <c r="D132" s="5"/>
       <c r="E132" s="5"/>
-      <c r="G132" s="5"/>
-    </row>
-    <row r="133" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="G132" s="9"/>
+    </row>
+    <row r="133" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B133" s="8"/>
       <c r="C133" s="5"/>
       <c r="D133" s="5"/>
       <c r="E133" s="5"/>
       <c r="G133" s="5"/>
     </row>
-    <row r="134" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B134" s="8"/>
       <c r="C134" s="5"/>
       <c r="D134" s="5"/>
       <c r="E134" s="5"/>
       <c r="G134" s="5"/>
     </row>
-    <row r="135" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B135" s="8"/>
       <c r="C135" s="5"/>
       <c r="D135" s="5"/>
       <c r="E135" s="5"/>
       <c r="G135" s="5"/>
     </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B136" s="8"/>
-      <c r="C136" s="10"/>
+      <c r="C136" s="5"/>
       <c r="D136" s="5"/>
       <c r="E136" s="5"/>
-      <c r="F136" s="7"/>
       <c r="G136" s="5"/>
     </row>
-    <row r="137" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B137" s="8"/>
-      <c r="C137" s="10"/>
+      <c r="C137" s="5"/>
       <c r="D137" s="5"/>
       <c r="E137" s="5"/>
       <c r="G137" s="5"/>
     </row>
-    <row r="138" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B138" s="8"/>
       <c r="C138" s="10"/>
       <c r="D138" s="5"/>
       <c r="E138" s="5"/>
+      <c r="F138" s="7"/>
       <c r="G138" s="5"/>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B139" s="8"/>
+      <c r="C139" s="10"/>
       <c r="D139" s="5"/>
       <c r="E139" s="5"/>
-      <c r="F139" s="7"/>
       <c r="G139" s="5"/>
     </row>
-    <row r="140" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B140" s="8"/>
-      <c r="C140" s="5"/>
+      <c r="C140" s="10"/>
       <c r="D140" s="5"/>
       <c r="E140" s="5"/>
       <c r="G140" s="5"/>
     </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B141" s="8"/>
       <c r="D141" s="5"/>
       <c r="E141" s="5"/>
       <c r="F141" s="7"/>
       <c r="G141" s="5"/>
     </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B142" s="8"/>
+      <c r="C142" s="5"/>
       <c r="D142" s="5"/>
       <c r="E142" s="5"/>
-      <c r="F142" s="7"/>
       <c r="G142" s="5"/>
     </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B143" s="8"/>
       <c r="D143" s="5"/>
       <c r="E143" s="5"/>
       <c r="F143" s="7"/>
       <c r="G143" s="5"/>
     </row>
-    <row r="144" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B144" s="8"/>
-      <c r="C144" s="5"/>
       <c r="D144" s="5"/>
       <c r="E144" s="5"/>
+      <c r="F144" s="7"/>
       <c r="G144" s="5"/>
     </row>
-    <row r="145" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B145" s="8"/>
-      <c r="C145" s="5"/>
       <c r="D145" s="5"/>
       <c r="E145" s="5"/>
+      <c r="F145" s="7"/>
       <c r="G145" s="5"/>
     </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B146" s="8"/>
+      <c r="C146" s="5"/>
       <c r="D146" s="5"/>
       <c r="E146" s="5"/>
-      <c r="F146" s="7"/>
       <c r="G146" s="5"/>
     </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B147" s="8"/>
+      <c r="C147" s="5"/>
       <c r="D147" s="5"/>
       <c r="E147" s="5"/>
-      <c r="F147" s="7"/>
       <c r="G147" s="5"/>
     </row>
-    <row r="148" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B148" s="8"/>
-      <c r="C148" s="5"/>
       <c r="D148" s="5"/>
       <c r="E148" s="5"/>
+      <c r="F148" s="7"/>
       <c r="G148" s="5"/>
     </row>
-    <row r="149" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B149" s="8"/>
-      <c r="C149" s="5"/>
       <c r="D149" s="5"/>
       <c r="E149" s="5"/>
+      <c r="F149" s="7"/>
       <c r="G149" s="5"/>
     </row>
-    <row r="150" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B150" s="8"/>
       <c r="C150" s="5"/>
       <c r="D150" s="5"/>
       <c r="E150" s="5"/>
       <c r="G150" s="5"/>
     </row>
-    <row r="151" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B151" s="8"/>
       <c r="C151" s="5"/>
       <c r="D151" s="5"/>
       <c r="E151" s="5"/>
       <c r="G151" s="5"/>
     </row>
-    <row r="152" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B152" s="8"/>
       <c r="C152" s="5"/>
       <c r="D152" s="5"/>
       <c r="E152" s="5"/>
       <c r="G152" s="5"/>
     </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B153" s="2"/>
-      <c r="F153" s="7"/>
-    </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B154" s="2"/>
-      <c r="F154" s="7"/>
-    </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B153" s="8"/>
+      <c r="C153" s="5"/>
+      <c r="D153" s="5"/>
+      <c r="E153" s="5"/>
+      <c r="G153" s="5"/>
+    </row>
+    <row r="154" spans="2:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B154" s="8"/>
+      <c r="C154" s="5"/>
+      <c r="D154" s="5"/>
+      <c r="E154" s="5"/>
+      <c r="G154" s="5"/>
+    </row>
+    <row r="155" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B155" s="2"/>
       <c r="F155" s="7"/>
     </row>
-    <row r="156" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B156" s="2"/>
       <c r="F156" s="7"/>
     </row>
-    <row r="157" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B157" s="2"/>
       <c r="F157" s="7"/>
     </row>
-    <row r="158" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B158" s="2"/>
       <c r="F158" s="7"/>
     </row>
-    <row r="159" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B159" s="2"/>
       <c r="F159" s="7"/>
     </row>
-    <row r="160" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B160" s="2"/>
       <c r="F160" s="7"/>
     </row>
-    <row r="161" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B161" s="2"/>
       <c r="F161" s="7"/>
     </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B162" s="2"/>
       <c r="F162" s="7"/>
     </row>
-    <row r="163" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B163" s="2"/>
       <c r="F163" s="7"/>
     </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B164" s="2"/>
       <c r="F164" s="7"/>
     </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B165" s="2"/>
       <c r="F165" s="7"/>
     </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B166" s="2"/>
       <c r="F166" s="7"/>
     </row>
-    <row r="167" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B167" s="2"/>
       <c r="F167" s="7"/>
     </row>
-    <row r="168" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B168" s="2"/>
-      <c r="C168" s="5"/>
-    </row>
-    <row r="169" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F168" s="7"/>
+    </row>
+    <row r="169" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B169" s="2"/>
       <c r="F169" s="7"/>
     </row>
-    <row r="170" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B170" s="2"/>
-      <c r="F170" s="7"/>
-    </row>
-    <row r="171" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C170" s="5"/>
+    </row>
+    <row r="171" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B171" s="2"/>
-      <c r="C171" s="5"/>
-    </row>
-    <row r="172" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F171" s="7"/>
+    </row>
+    <row r="172" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B172" s="2"/>
-      <c r="C172" s="5"/>
-    </row>
-    <row r="173" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F172" s="7"/>
+    </row>
+    <row r="173" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B173" s="2"/>
-      <c r="D173" s="5"/>
-      <c r="E173" s="5"/>
-      <c r="F173" s="7"/>
-    </row>
-    <row r="174" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C173" s="5"/>
+    </row>
+    <row r="174" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B174" s="2"/>
-      <c r="F174" s="7"/>
-    </row>
-    <row r="175" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="C174" s="5"/>
+    </row>
+    <row r="175" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B175" s="2"/>
+      <c r="D175" s="5"/>
+      <c r="E175" s="5"/>
       <c r="F175" s="7"/>
     </row>
-    <row r="176" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B176" s="2"/>
       <c r="F176" s="7"/>
     </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="177" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B177" s="2"/>
       <c r="F177" s="7"/>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="178" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B178" s="2"/>
       <c r="F178" s="7"/>
     </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B179" s="2"/>
       <c r="F179" s="7"/>
     </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="180" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B180" s="2"/>
       <c r="F180" s="7"/>
     </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="181" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B181" s="2"/>
       <c r="F181" s="7"/>
     </row>
-    <row r="182" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B182" s="2"/>
       <c r="F182" s="7"/>
     </row>
-    <row r="183" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="183" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B183" s="2"/>
       <c r="F183" s="7"/>
     </row>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="184" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B184" s="2"/>
       <c r="F184" s="7"/>
     </row>
-    <row r="185" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B185" s="2"/>
-      <c r="C185" s="5"/>
-      <c r="D185" s="5"/>
-      <c r="E185" s="5"/>
+      <c r="F185" s="7"/>
+    </row>
+    <row r="186" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B186" s="2"/>
+      <c r="F186" s="7"/>
+    </row>
+    <row r="187" spans="2:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B187" s="2"/>
+      <c r="C187" s="5"/>
+      <c r="D187" s="5"/>
+      <c r="E187" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:G185">
+  <autoFilter ref="B1:G187">
     <sortState ref="B2:L87">
       <sortCondition ref="E1:E87"/>
     </sortState>
@@ -2210,7 +2263,7 @@
           <x14:formula1>
             <xm:f>Stats!$A$2:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>D110:D185 D2:D101</xm:sqref>
+          <xm:sqref>D112:D187 D2:D103</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2227,20 +2280,20 @@
       <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="7" customWidth="1"/>
-    <col min="2" max="2" width="8.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.26953125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="31.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48.1796875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="7"/>
+    <col min="2" max="2" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -2269,317 +2322,317 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="8"/>
       <c r="C2" s="5"/>
       <c r="F2" s="7"/>
       <c r="G2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
       <c r="C3" s="5"/>
       <c r="F3" s="7"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
       <c r="C4" s="5"/>
       <c r="F4" s="7"/>
       <c r="G4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="5"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="5"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="8"/>
       <c r="C8" s="5"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
       <c r="C9" s="5"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
       <c r="C10" s="5"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
       <c r="C11" s="5"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
       <c r="C13" s="5"/>
       <c r="F13"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="8"/>
       <c r="C14" s="5"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
       <c r="C15" s="5"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="8"/>
       <c r="C16" s="5"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="8"/>
       <c r="C17" s="5"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
       <c r="C18" s="5"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
       <c r="C19" s="5"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="8"/>
       <c r="C20" s="5"/>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="8"/>
       <c r="C21" s="5"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="8"/>
       <c r="C22" s="5"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
       <c r="C23" s="5"/>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
       <c r="C24" s="5"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="8"/>
       <c r="C25" s="5"/>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>
       <c r="C26" s="5"/>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
       <c r="C27" s="5"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="8"/>
       <c r="C28" s="5"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="8"/>
       <c r="C29" s="5"/>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
       <c r="C30" s="5"/>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
       <c r="C31" s="10"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="8"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="5"/>
       <c r="D33" s="7"/>
       <c r="E33" s="5"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="5"/>
       <c r="D34" s="7"/>
       <c r="E34" s="5"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="5"/>
       <c r="D35" s="7"/>
       <c r="E35" s="5"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="5"/>
       <c r="D36" s="7"/>
       <c r="E36" s="5"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="5"/>
       <c r="D37" s="7"/>
       <c r="E37" s="5"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="5"/>
       <c r="D38" s="7"/>
       <c r="E38" s="5"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="5"/>
       <c r="D39" s="7"/>
       <c r="E39" s="5"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="5"/>
       <c r="D40" s="7"/>
       <c r="E40" s="5"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="5"/>
       <c r="D41" s="7"/>
       <c r="E41" s="5"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="5"/>
       <c r="D42" s="7"/>
       <c r="E42" s="5"/>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="5"/>
       <c r="D43" s="7"/>
       <c r="E43" s="5"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="5"/>
       <c r="D44" s="7"/>
       <c r="E44" s="5"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="5"/>
       <c r="D45" s="7"/>
       <c r="E45" s="5"/>
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="5"/>
       <c r="D46" s="7"/>
       <c r="E46" s="5"/>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="5"/>
       <c r="D47" s="7"/>
       <c r="E47" s="5"/>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="5"/>
       <c r="D48" s="7"/>
       <c r="E48" s="5"/>
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="5"/>
       <c r="D49" s="7"/>
       <c r="E49" s="5"/>
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="5"/>
       <c r="D50" s="7"/>
       <c r="E50" s="5"/>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="5"/>
       <c r="D51" s="7"/>
       <c r="E51" s="5"/>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="5"/>
       <c r="D52" s="7"/>
       <c r="E52" s="5"/>
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="5"/>
       <c r="D53" s="7"/>
       <c r="E53" s="5"/>
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="5"/>
       <c r="D54" s="7"/>
       <c r="E54" s="5"/>
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="55" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2612,19 +2665,19 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7265625" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -2650,15 +2703,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>56</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>15</v>
@@ -2667,117 +2720,117 @@
         <v>39</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G2" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>59</v>
-      </c>
       <c r="C3" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G3" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>63</v>
-      </c>
       <c r="F4" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G4" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>67</v>
       </c>
       <c r="G5" s="7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G6" s="7" t="b">
         <v>0</v>
       </c>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
     </row>
-    <row r="8" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
     </row>
-    <row r="9" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
     </row>
-    <row r="10" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -2793,23 +2846,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6:E17"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="A2:C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="92" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" style="7" customWidth="1"/>
-    <col min="5" max="9" width="11.7265625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="7" customWidth="1"/>
+    <col min="5" max="9" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -2838,7 +2891,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <f>Achievements!A2</f>
         <v>1</v>
@@ -2863,12 +2916,15 @@
       <c r="G2" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H2" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I2" s="7" t="str">
         <f t="shared" ref="I2:I4" si="0">IF(COUNTIF(D2:H2,"X")=5,"YES","NO")</f>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <f>Achievements!A3</f>
         <v>2</v>
@@ -2893,12 +2949,15 @@
       <c r="G3" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H3" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I3" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <f>Achievements!A4</f>
         <v>3</v>
@@ -2923,23 +2982,26 @@
       <c r="G4" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H4" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I4" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <f>Achievements!A5</f>
         <v>4</v>
       </c>
       <c r="B5" s="7" t="str">
         <f>Achievements!C5</f>
-        <v>Tough as Nails</v>
+        <v>Sergeant Major</v>
       </c>
       <c r="C5" s="7" t="str">
         <f>Achievements!F5</f>
-        <v>Score 10,000 without dying</v>
+        <v>Score 100,000</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>20</v>
@@ -2953,23 +3015,26 @@
       <c r="G5" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="H5" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I5" s="7" t="str">
-        <f t="shared" ref="I5:I12" si="1">IF(COUNTIF(D5:H5,"X")=5,"YES","NO")</f>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <f t="shared" ref="I5:I25" si="1">IF(COUNTIF(D5:H5,"X")=5,"YES","NO")</f>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <f>Achievements!A6</f>
         <v>5</v>
       </c>
       <c r="B6" s="7" t="str">
         <f>Achievements!C6</f>
-        <v>One-Man Army</v>
+        <v>Tough as Nails</v>
       </c>
       <c r="C6" s="7" t="str">
         <f>Achievements!F6</f>
-        <v>Score 25,000 without dying</v>
+        <v>Score 10,000 without dying</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>20</v>
@@ -2983,24 +3048,26 @@
       <c r="G6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I6" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <f>Achievements!A7</f>
         <v>6</v>
       </c>
       <c r="B7" s="7" t="str">
         <f>Achievements!C7</f>
-        <v>Finely Tuned</v>
+        <v>One-Man Army</v>
       </c>
       <c r="C7" s="7" t="str">
         <f>Achievements!F7</f>
-        <v>Reach the final speed up phase in mode 1</v>
+        <v>Score 25,000 without dying</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>20</v>
@@ -3014,24 +3081,26 @@
       <c r="G7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I7" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <f>Achievements!A8</f>
         <v>7</v>
       </c>
       <c r="B8" s="7" t="str">
         <f>Achievements!C8</f>
-        <v>Broad Strokes</v>
+        <v>Indestructible</v>
       </c>
       <c r="C8" s="7" t="str">
         <f>Achievements!F8</f>
-        <v>Reach the final speed up phase in mode 2</v>
+        <v>Score 25,000 without dying</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>20</v>
@@ -3045,24 +3114,26 @@
       <c r="G8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I8" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <f>Achievements!A9</f>
         <v>8</v>
       </c>
       <c r="B9" s="7" t="str">
         <f>Achievements!C9</f>
-        <v>Fear of the Dark</v>
+        <v>Finely Tuned</v>
       </c>
       <c r="C9" s="7" t="str">
         <f>Achievements!F9</f>
-        <v>Reach the final speed up phase in mode 3</v>
+        <v>Reach the final speed up phase in mode 1</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>20</v>
@@ -3076,24 +3147,26 @@
       <c r="G9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <f>Achievements!A10</f>
         <v>9</v>
       </c>
       <c r="B10" s="7" t="str">
         <f>Achievements!C10</f>
-        <v>Jeep Tricks</v>
+        <v>Broad Strokes</v>
       </c>
       <c r="C10" s="7" t="str">
         <f>Achievements!F10</f>
-        <v>Gain a life</v>
+        <v>Reach the final speed up phase in mode 2</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>20</v>
@@ -3105,25 +3178,28 @@
         <v>20</v>
       </c>
       <c r="G10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I10" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <f>Achievements!A11</f>
         <v>10</v>
       </c>
       <c r="B11" s="7" t="str">
         <f>Achievements!C11</f>
-        <v>King of the Hill</v>
+        <v>Fear of the Dark</v>
       </c>
       <c r="C11" s="7" t="str">
         <f>Achievements!F11</f>
-        <v>Survive in the middle of the middle for 1 minute</v>
+        <v>Reach the final speed up phase in mode 3</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>20</v>
@@ -3135,25 +3211,28 @@
         <v>20</v>
       </c>
       <c r="G11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I11" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <f>Achievements!A12</f>
         <v>11</v>
       </c>
       <c r="B12" s="7" t="str">
         <f>Achievements!C12</f>
-        <v>King of the Mountain</v>
+        <v>Jeep Tricks</v>
       </c>
       <c r="C12" s="7" t="str">
         <f>Achievements!F12</f>
-        <v>Survive in the middle of the middle for 3 minutes</v>
+        <v>Gain a life</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>20</v>
@@ -3167,24 +3246,26 @@
       <c r="G12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="7"/>
+      <c r="H12" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I12" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <f>Achievements!A13</f>
         <v>12</v>
       </c>
       <c r="B13" s="7" t="str">
         <f>Achievements!C13</f>
-        <v>Happy Camper</v>
+        <v>King of the Hill</v>
       </c>
       <c r="C13" s="7" t="str">
         <f>Achievements!F13</f>
-        <v>Survive without moving for 1 minute</v>
+        <v>Survive in the middle of the middle for 1 minute</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>20</v>
@@ -3198,24 +3279,26 @@
       <c r="G13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I13" s="7" t="str">
-        <f t="shared" ref="I13:I23" si="2">IF(COUNTIF(D13:H13,"X")=5,"YES","NO")</f>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <f>Achievements!A14</f>
         <v>13</v>
       </c>
       <c r="B14" s="7" t="str">
         <f>Achievements!C14</f>
-        <v>Wilderness Survival</v>
+        <v>King of the Mountain</v>
       </c>
       <c r="C14" s="7" t="str">
         <f>Achievements!F14</f>
-        <v>Survive without moving for 3 minutes</v>
+        <v>Survive in the middle of the middle for 3 minutes</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>20</v>
@@ -3229,24 +3312,26 @@
       <c r="G14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="7"/>
+      <c r="H14" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I14" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <f>Achievements!A15</f>
         <v>14</v>
       </c>
       <c r="B15" s="7" t="str">
         <f>Achievements!C15</f>
-        <v>Armor Pacifist</v>
+        <v>Happy Camper</v>
       </c>
       <c r="C15" s="7" t="str">
         <f>Achievements!F15</f>
-        <v>Survive without destroying an enemy for 1 minute</v>
+        <v>Survive without moving for 1 minute</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>20</v>
@@ -3260,24 +3345,26 @@
       <c r="G15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="7"/>
+      <c r="H15" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I15" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <f>Achievements!A16</f>
         <v>15</v>
       </c>
       <c r="B16" s="7" t="str">
         <f>Achievements!C16</f>
-        <v>Peace Keeper</v>
+        <v>Wilderness Survival</v>
       </c>
       <c r="C16" s="7" t="str">
         <f>Achievements!F16</f>
-        <v>Survive without destroying an enemy for 3 minutes</v>
+        <v>Survive without moving for 3 minutes</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>20</v>
@@ -3291,24 +3378,26 @@
       <c r="G16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="7"/>
+      <c r="H16" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I16" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <f>Achievements!A17</f>
         <v>16</v>
       </c>
       <c r="B17" s="7" t="str">
         <f>Achievements!C17</f>
-        <v>Friendly Fire</v>
+        <v>Armor Pacifist</v>
       </c>
       <c r="C17" s="7" t="str">
         <f>Achievements!F17</f>
-        <v>Let an enemy damage or destroy another tank 25 times</v>
+        <v>Survive without destroying an enemy for 1 minute</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>20</v>
@@ -3322,229 +3411,321 @@
       <c r="G17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I17" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <f>Achievements!A18</f>
         <v>17</v>
       </c>
       <c r="B18" s="7" t="str">
         <f>Achievements!C18</f>
-        <v>Tanks for Nothing!</v>
+        <v>Peace Keeper</v>
       </c>
       <c r="C18" s="7" t="str">
         <f>Achievements!F18</f>
-        <v>Fully destroy 10 tanks (requires two shots)</v>
+        <v>Survive without destroying an enemy for 3 minutes</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="7"/>
+      <c r="E18" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="F18" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="7"/>
+      <c r="H18" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I18" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <f>Achievements!A19</f>
         <v>18</v>
       </c>
       <c r="B19" s="7" t="str">
         <f>Achievements!C19</f>
-        <v>Go Get 'em Tiger!</v>
+        <v>Friendly Fire</v>
       </c>
       <c r="C19" s="7" t="str">
         <f>Achievements!F19</f>
-        <v>Fully destroy 25 tanks (requires two shots)</v>
+        <v>Let an enemy damage or destroy another tank 25 times</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="7"/>
+      <c r="E19" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="F19" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="7"/>
+      <c r="H19" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I19" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <f>Achievements!A20</f>
         <v>19</v>
       </c>
       <c r="B20" s="7" t="str">
         <f>Achievements!C20</f>
-        <v>Doom Turtles All the Way Down!</v>
+        <v>Tanks for Nothing!</v>
       </c>
       <c r="C20" s="7" t="str">
         <f>Achievements!F20</f>
-        <v>Fully destroy 50 tanks (requires two shots)</v>
+        <v>Fully destroy 10 tanks (requires two shots)</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="7"/>
+      <c r="E20" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="F20" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="7"/>
+      <c r="H20" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I20" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <f>Achievements!A21</f>
         <v>20</v>
       </c>
       <c r="B21" s="7" t="str">
         <f>Achievements!C21</f>
-        <v>Get to the Chopper!</v>
+        <v>Go Get 'em Tiger!</v>
       </c>
       <c r="C21" s="7" t="str">
         <f>Achievements!F21</f>
-        <v>Destroy 6 Helicoptors</v>
+        <v>Fully destroy 20 tanks (requires two shots)</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="7"/>
+      <c r="E21" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="F21" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="7"/>
+      <c r="H21" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I21" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <f>Achievements!A22</f>
         <v>21</v>
       </c>
       <c r="B22" s="7" t="str">
         <f>Achievements!C22</f>
-        <v>Whirlybird Wrecked!</v>
+        <v>Doom Turtles All the Way Down!</v>
       </c>
       <c r="C22" s="7" t="str">
         <f>Achievements!F22</f>
-        <v>Destroy 12 Helicoptors</v>
+        <v>Fully destroy 30 tanks (requires two shots)</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="7"/>
+      <c r="E22" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="F22" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="7"/>
+      <c r="H22" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="I22" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <f>Achievements!A23</f>
         <v>22</v>
       </c>
       <c r="B23" s="7" t="str">
         <f>Achievements!C23</f>
-        <v>Blackhawk Down!</v>
+        <v>Aerial Attack!</v>
       </c>
       <c r="C23" s="7" t="str">
         <f>Achievements!F23</f>
+        <v>Destroy 6 Helicoptors</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <f>Achievements!A24</f>
+        <v>23</v>
+      </c>
+      <c r="B24" s="7" t="str">
+        <f>Achievements!C24</f>
+        <v>Whirlybird Wrecked!</v>
+      </c>
+      <c r="C24" s="7" t="str">
+        <f>Achievements!F24</f>
+        <v>Destroy 12 Helicoptors</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <f>Achievements!A25</f>
+        <v>24</v>
+      </c>
+      <c r="B25" s="7" t="str">
+        <f>Achievements!C25</f>
+        <v>Blackhawk Down!</v>
+      </c>
+      <c r="C25" s="7" t="str">
+        <f>Achievements!F25</f>
         <v>Destroy 24 Helicoptors</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7" t="str">
+      <c r="D25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>YES</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7" t="str">
+        <f t="shared" ref="D26:G26" si="2">COUNTIF(D2:D25,"X")&amp;" /24"</f>
+        <v>24 /24</v>
+      </c>
+      <c r="E26" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7" t="str">
-        <f t="shared" ref="D24:I24" si="3">COUNTIF(D2:D23,"X")&amp;" /22"</f>
-        <v>22 /22</v>
-      </c>
-      <c r="E24" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>16 /22</v>
-      </c>
-      <c r="F24" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>22 /22</v>
-      </c>
-      <c r="G24" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>22 /22</v>
-      </c>
-      <c r="H24" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>0 /22</v>
-      </c>
-      <c r="I24" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>0 /22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B26" s="7"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+        <v>24 /24</v>
+      </c>
+      <c r="F26" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>24 /24</v>
+      </c>
+      <c r="G26" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>24 /24</v>
+      </c>
+      <c r="H26" s="7" t="str">
+        <f>COUNTIF(H2:H25,"X")&amp;" /24"</f>
+        <v>24 /24</v>
+      </c>
+      <c r="I26" s="7" t="str">
+        <f>COUNTIF(I2:I25,"YES")&amp;" /24"</f>
+        <v>24 /24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1">
@@ -3565,460 +3746,460 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="129.453125" customWidth="1"/>
+    <col min="1" max="1" width="129.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="str">
         <f ca="1">"achievement("&amp;CHAR(34)&amp;INDIRECT("Achievements!C"&amp;(ROW()-1))&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;INDIRECT("Achievements!F"&amp;(ROW()-1))&amp;CHAR(34)&amp;", "&amp;INDIRECT("Achievements!E"&amp;(ROW()-1))&amp;", trigger)"</f>
         <v>achievement("Private","Score 10,000", 3, trigger)</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="str">
         <f t="shared" ref="A4:A24" ca="1" si="0">"achievement("&amp;CHAR(34)&amp;INDIRECT("Achievements!C"&amp;(ROW()-1))&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;INDIRECT("Achievements!F"&amp;(ROW()-1))&amp;CHAR(34)&amp;", "&amp;INDIRECT("Achievements!E"&amp;(ROW()-1))&amp;", trigger)"</f>
         <v>achievement("Corporal ","Score 25,000", 5, trigger)</v>
       </c>
     </row>
-    <row r="5" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>achievement("Sergeant ","Score 50,000", 10, trigger)</v>
       </c>
     </row>
-    <row r="6" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Tough as Nails","Score 10,000 without dying", 5, trigger)</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Sergeant Major","Score 100,000", 25, trigger)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("One-Man Army","Score 25,000 without dying", 10, trigger)</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Tough as Nails","Score 10,000 without dying", 5, trigger)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Finely Tuned","Reach the final speed up phase in mode 1", 5, trigger)</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("One-Man Army","Score 25,000 without dying", 10, trigger)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Broad Strokes","Reach the final speed up phase in mode 2", 5, trigger)</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Indestructible","Score 25,000 without dying", 10, trigger)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Fear of the Dark","Reach the final speed up phase in mode 3", 5, trigger)</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Finely Tuned","Reach the final speed up phase in mode 1", 5, trigger)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Jeep Tricks","Gain a life", 5, trigger)</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Broad Strokes","Reach the final speed up phase in mode 2", 5, trigger)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("King of the Hill","Survive in the middle of the middle for 1 minute", 3, trigger)</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Fear of the Dark","Reach the final speed up phase in mode 3", 5, trigger)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("King of the Mountain","Survive in the middle of the middle for 3 minutes", 5, trigger)</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Jeep Tricks","Gain a life", 5, trigger)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Happy Camper","Survive without moving for 1 minute", 2, trigger)</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("King of the Hill","Survive in the middle of the middle for 1 minute", 3, trigger)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Wilderness Survival","Survive without moving for 3 minutes", 5, trigger)</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("King of the Mountain","Survive in the middle of the middle for 3 minutes", 5, trigger)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Armor Pacifist","Survive without destroying an enemy for 1 minute", 2, trigger)</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Happy Camper","Survive without moving for 1 minute", 2, trigger)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Peace Keeper","Survive without destroying an enemy for 3 minutes", 5, trigger)</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Wilderness Survival","Survive without moving for 3 minutes", 5, trigger)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="str">
         <f ca="1">"achievement("&amp;CHAR(34)&amp;INDIRECT("Achievements!C"&amp;(ROW()-1))&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;INDIRECT("Achievements!F"&amp;(ROW()-1))&amp;CHAR(34)&amp;", "&amp;INDIRECT("Achievements!E"&amp;(ROW()-1))&amp;", trigger)"</f>
-        <v>achievement("Friendly Fire","Let an enemy damage or destroy another tank 25 times", 5, trigger)</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Armor Pacifist","Survive without destroying an enemy for 1 minute", 2, trigger)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Tanks for Nothing!","Fully destroy 10 tanks (requires two shots)", 2, trigger)</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Peace Keeper","Survive without destroying an enemy for 3 minutes", 5, trigger)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Go Get 'em Tiger!","Fully destroy 25 tanks (requires two shots)", 3, trigger)</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Friendly Fire","Let an enemy damage or destroy another tank 25 times", 5, trigger)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Doom Turtles All the Way Down!","Fully destroy 50 tanks (requires two shots)", 5, trigger)</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Tanks for Nothing!","Fully destroy 10 tanks (requires two shots)", 2, trigger)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Get to the Chopper!","Destroy 6 Helicoptors", 2, trigger)</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Go Get 'em Tiger!","Fully destroy 20 tanks (requires two shots)", 3, trigger)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Whirlybird Wrecked!","Destroy 12 Helicoptors", 3, trigger)</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Doom Turtles All the Way Down!","Fully destroy 30 tanks (requires two shots)", 5, trigger)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>achievement("Blackhawk Down!","Destroy 24 Helicoptors", 5, trigger)</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Aerial Attack!","Destroy 6 Helicoptors", 2, trigger)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="str">
         <f t="shared" ref="A25:A67" ca="1" si="1">"achievement("&amp;CHAR(34)&amp;INDIRECT("Achievements!C"&amp;(ROW()-1))&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;INDIRECT("Achievements!H"&amp;(ROW()-1))&amp;CHAR(34)&amp;", "&amp;INDIRECT("Achievements!E"&amp;(ROW()-1))&amp;", trigger)"</f>
-        <v>achievement("","", , trigger)</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Whirlybird Wrecked!","", 3, trigger)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>achievement("","", , trigger)</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>achievement("Blackhawk Down!","", 5, trigger)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="28" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="29" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="30" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="31" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="32" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="33" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="34" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="35" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="36" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="37" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="38" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="39" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>achievement("","", 100, trigger)</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+        <v>achievement("","", , trigger)</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>achievement("","", , trigger)</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+        <v>achievement("","", 135, trigger)</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="57" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="str">
         <f t="shared" ref="A68:A76" ca="1" si="2">"achievement("&amp;CHAR(34)&amp;INDIRECT("Achievements!C"&amp;(ROW()-1))&amp;CHAR(34)&amp;","&amp;CHAR(34)&amp;INDIRECT("Achievements!H"&amp;(ROW()-1))&amp;CHAR(34)&amp;", "&amp;INDIRECT("Achievements!E"&amp;(ROW()-1))&amp;", trigger)"</f>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>achievement("","", , trigger)</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>achievement("","", , trigger)</v>
@@ -4039,13 +4220,13 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>35</v>
       </c>
@@ -4066,7 +4247,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -4090,7 +4271,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -4106,15 +4287,15 @@
       </c>
       <c r="F3" s="4">
         <f>COUNTIF(Achievements!B:B,E3)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3" s="7">
         <f>SUMIF(Achievements!B:B,E3,Achievements!E:E)</f>
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -4130,14 +4311,14 @@
       </c>
       <c r="F4" s="4">
         <f>COUNTIF(Achievements!B:B,E4)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="7">
         <f>SUMIF(Achievements!B:B,E4,Achievements!E:E)</f>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -4160,7 +4341,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -4176,14 +4357,14 @@
       </c>
       <c r="F6" s="3">
         <f>SUM(F2:F5)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G6" s="3">
         <f>SUM(G2:G5)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4195,7 +4376,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -4204,10 +4385,10 @@
       </c>
       <c r="C8">
         <f>COUNTIF(Achievements!D:D,A8)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
@@ -4216,10 +4397,10 @@
       </c>
       <c r="C9" s="7">
         <f>COUNTIF(Achievements!D:D,A9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -4231,14 +4412,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3">
         <f>SUM(C2:C10)</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -4254,13 +4435,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="21" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -4326,7 +4507,7 @@
       </c>
       <c r="V1" s="7"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4411,7 +4592,7 @@
       </c>
       <c r="V2" s="7"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4496,7 +4677,7 @@
         <v>38963</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4581,7 +4762,7 @@
         <v>38995</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4666,7 +4847,7 @@
         <v>39027</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4751,7 +4932,7 @@
         <v>39059</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4836,7 +5017,7 @@
         <v>39091</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -4921,7 +5102,7 @@
         <v>39123</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -5006,7 +5187,7 @@
         <v>39155</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -5091,7 +5272,7 @@
         <v>39187</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -5176,7 +5357,7 @@
         <v>39219</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>10</v>
       </c>
@@ -5261,7 +5442,7 @@
         <v>39251</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -5346,7 +5527,7 @@
         <v>39283</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>12</v>
       </c>
@@ -5431,7 +5612,7 @@
         <v>39315</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>13</v>
       </c>
@@ -5516,7 +5697,7 @@
         <v>39347</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>14</v>
       </c>
@@ -5601,7 +5782,7 @@
         <v>39379</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>15</v>
       </c>
@@ -5686,7 +5867,7 @@
         <v>39411</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>16</v>
       </c>
@@ -5771,7 +5952,7 @@
         <v>39443</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>17</v>
       </c>
@@ -5856,7 +6037,7 @@
         <v>39475</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>18</v>
       </c>
@@ -5941,7 +6122,7 @@
         <v>39507</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>19</v>
       </c>
@@ -6026,7 +6207,7 @@
         <v>39539</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
     </row>
   </sheetData>

</xml_diff>